<commit_message>
Found potential issue with installing Zero2Go software.
</commit_message>
<xml_diff>
--- a/documentation/build.xlsx
+++ b/documentation/build.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ian\Documents\GitHub\Corona_Cam\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ian\Documents\GitHub\corona_cam\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8AF36D8-6668-4F29-B950-BCF14A73E592}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA234234-D3F6-4B8F-8818-891872158AC3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{BFA8654B-9BE4-4811-B5B6-CC71729ADED4}"/>
   </bookViews>
@@ -938,6 +938,18 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -963,18 +975,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1296,7 +1296,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G26" sqref="G26"/>
+      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1317,9 +1317,9 @@
       <c r="A1" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="90">
+      <c r="B1" s="81">
         <f>SUM(F4:F25)</f>
-        <v>347.95</v>
+        <v>350.9</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="5"/>
@@ -1355,16 +1355,16 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="18" x14ac:dyDescent="0.3">
-      <c r="A3" s="91" t="s">
+      <c r="A3" s="82" t="s">
         <v>92</v>
       </c>
-      <c r="B3" s="92"/>
-      <c r="C3" s="92"/>
-      <c r="D3" s="92"/>
-      <c r="E3" s="92"/>
-      <c r="F3" s="92"/>
-      <c r="G3" s="92"/>
-      <c r="H3" s="93"/>
+      <c r="B3" s="83"/>
+      <c r="C3" s="83"/>
+      <c r="D3" s="83"/>
+      <c r="E3" s="83"/>
+      <c r="F3" s="83"/>
+      <c r="G3" s="83"/>
+      <c r="H3" s="84"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
@@ -1505,11 +1505,11 @@
         <v>2.95</v>
       </c>
       <c r="E9" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F9" s="7">
         <f t="shared" si="0"/>
-        <v>2.95</v>
+        <v>5.9</v>
       </c>
       <c r="G9" s="23" t="s">
         <v>78</v>
@@ -1916,16 +1916,16 @@
     </row>
     <row r="26" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="27" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="87" t="s">
+      <c r="A27" s="91" t="s">
         <v>39</v>
       </c>
-      <c r="B27" s="88"/>
-      <c r="C27" s="88"/>
-      <c r="D27" s="88"/>
-      <c r="E27" s="88"/>
-      <c r="F27" s="88"/>
-      <c r="G27" s="88"/>
-      <c r="H27" s="89"/>
+      <c r="B27" s="92"/>
+      <c r="C27" s="92"/>
+      <c r="D27" s="92"/>
+      <c r="E27" s="92"/>
+      <c r="F27" s="92"/>
+      <c r="G27" s="92"/>
+      <c r="H27" s="93"/>
     </row>
     <row r="28" spans="1:8" ht="18" x14ac:dyDescent="0.3">
       <c r="A28" s="49" t="s">
@@ -2011,16 +2011,16 @@
     </row>
     <row r="33" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="34" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="81" t="s">
+      <c r="A34" s="85" t="s">
         <v>40</v>
       </c>
-      <c r="B34" s="82"/>
-      <c r="C34" s="82"/>
-      <c r="D34" s="82"/>
-      <c r="E34" s="82"/>
-      <c r="F34" s="82"/>
-      <c r="G34" s="82"/>
-      <c r="H34" s="83"/>
+      <c r="B34" s="86"/>
+      <c r="C34" s="86"/>
+      <c r="D34" s="86"/>
+      <c r="E34" s="86"/>
+      <c r="F34" s="86"/>
+      <c r="G34" s="86"/>
+      <c r="H34" s="87"/>
     </row>
     <row r="35" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A35" s="60" t="s">
@@ -2102,16 +2102,16 @@
     </row>
     <row r="40" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="41" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="84" t="s">
+      <c r="A41" s="88" t="s">
         <v>48</v>
       </c>
-      <c r="B41" s="85"/>
-      <c r="C41" s="85"/>
-      <c r="D41" s="85"/>
-      <c r="E41" s="85"/>
-      <c r="F41" s="85"/>
-      <c r="G41" s="85"/>
-      <c r="H41" s="86"/>
+      <c r="B41" s="89"/>
+      <c r="C41" s="89"/>
+      <c r="D41" s="89"/>
+      <c r="E41" s="89"/>
+      <c r="F41" s="89"/>
+      <c r="G41" s="89"/>
+      <c r="H41" s="90"/>
     </row>
     <row r="42" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A42" s="70" t="s">

</xml_diff>

<commit_message>
Removed references to the Zero2Go Omini.
It it too frustrating to use.
</commit_message>
<xml_diff>
--- a/documentation/build.xlsx
+++ b/documentation/build.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ian\Documents\GitHub\corona_cam\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA234234-D3F6-4B8F-8818-891872158AC3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBCD36E8-699C-41E9-877C-4F1883A2D319}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{BFA8654B-9BE4-4811-B5B6-CC71729ADED4}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="108">
   <si>
     <t>Part</t>
   </si>
@@ -78,9 +78,6 @@
     <t>Adafruit PiRTC - DS3231</t>
   </si>
   <si>
-    <t>Zero2Go Omini Multi-Channel Power Supply</t>
-  </si>
-  <si>
     <t>Comment</t>
   </si>
   <si>
@@ -271,9 +268,6 @@
   </si>
   <si>
     <t>For keeping time.</t>
-  </si>
-  <si>
-    <t>For managing power.</t>
   </si>
   <si>
     <t>Dual o-ring seal against the tube.</t>
@@ -1292,11 +1286,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27939F0E-BC23-4F8A-AA1D-D2FCDAD892C2}">
-  <dimension ref="A1:H54"/>
+  <dimension ref="A1:H53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
+      <selection pane="bottomLeft" activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1315,11 +1309,11 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B1" s="81">
-        <f>SUM(F4:F25)</f>
-        <v>350.9</v>
+        <f>SUM(F4:F24)</f>
+        <v>330.95</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="5"/>
@@ -1348,7 +1342,7 @@
         <v>5</v>
       </c>
       <c r="G2" s="22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H2" s="11" t="s">
         <v>13</v>
@@ -1356,7 +1350,7 @@
     </row>
     <row r="3" spans="1:8" ht="18" x14ac:dyDescent="0.3">
       <c r="A3" s="82" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B3" s="83"/>
       <c r="C3" s="83"/>
@@ -1387,7 +1381,7 @@
         <v>10</v>
       </c>
       <c r="G4" s="23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H4" s="14"/>
     </row>
@@ -1408,11 +1402,11 @@
         <v>1</v>
       </c>
       <c r="F5" s="7">
-        <f t="shared" ref="F5:F25" si="0">D5*E5</f>
+        <f t="shared" ref="F5:F24" si="0">D5*E5</f>
         <v>11.95</v>
       </c>
       <c r="G5" s="23" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H5" s="14"/>
     </row>
@@ -1437,7 +1431,7 @@
         <v>4.5</v>
       </c>
       <c r="G6" s="23" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H6" s="14"/>
     </row>
@@ -1462,7 +1456,7 @@
         <v>5.95</v>
       </c>
       <c r="G7" s="23" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H7" s="14"/>
     </row>
@@ -1487,7 +1481,7 @@
         <v>2.5</v>
       </c>
       <c r="G8" s="23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H8" s="14"/>
     </row>
@@ -1512,7 +1506,7 @@
         <v>5.9</v>
       </c>
       <c r="G9" s="23" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H9" s="14"/>
     </row>
@@ -1537,435 +1531,424 @@
         <v>14.95</v>
       </c>
       <c r="G10" s="23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H10" s="14"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="13" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="6">
-        <v>4114</v>
+        <v>2141</v>
       </c>
       <c r="D11" s="7">
-        <v>19.95</v>
+        <v>2.75</v>
       </c>
       <c r="E11" s="6">
         <v>1</v>
       </c>
       <c r="F11" s="7">
         <f t="shared" si="0"/>
-        <v>19.95</v>
+        <v>2.75</v>
       </c>
       <c r="G11" s="23" t="s">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="H11" s="14"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="13" t="s">
-        <v>60</v>
+        <v>16</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="6">
-        <v>2141</v>
+        <v>17</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="D12" s="7">
-        <v>2.75</v>
+        <v>12.99</v>
       </c>
       <c r="E12" s="6">
         <v>1</v>
       </c>
       <c r="F12" s="7">
         <f t="shared" si="0"/>
-        <v>2.75</v>
+        <v>12.99</v>
       </c>
       <c r="G12" s="23" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="H12" s="14"/>
     </row>
-    <row r="13" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="6" t="s">
-        <v>18</v>
-      </c>
       <c r="C13" s="6" t="s">
-        <v>19</v>
+        <v>70</v>
       </c>
       <c r="D13" s="7">
-        <v>12.99</v>
+        <v>5.49</v>
       </c>
       <c r="E13" s="6">
         <v>1</v>
       </c>
       <c r="F13" s="7">
         <f t="shared" si="0"/>
-        <v>12.99</v>
+        <v>5.49</v>
       </c>
       <c r="G13" s="23" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H13" s="14"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A14" s="13" t="s">
-        <v>70</v>
+        <v>19</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>71</v>
+        <v>20</v>
       </c>
       <c r="D14" s="7">
-        <v>5.49</v>
+        <v>7.99</v>
       </c>
       <c r="E14" s="6">
         <v>1</v>
       </c>
       <c r="F14" s="7">
         <f t="shared" si="0"/>
-        <v>5.49</v>
+        <v>7.99</v>
       </c>
       <c r="G14" s="23" t="s">
-        <v>72</v>
+        <v>105</v>
       </c>
       <c r="H14" s="14"/>
     </row>
-    <row r="15" spans="1:8" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A15" s="13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>23</v>
       </c>
       <c r="D15" s="7">
-        <v>7.99</v>
+        <v>24</v>
       </c>
       <c r="E15" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F15" s="7">
         <f t="shared" si="0"/>
-        <v>7.99</v>
+        <v>48</v>
       </c>
       <c r="G15" s="23" t="s">
-        <v>107</v>
+        <v>79</v>
       </c>
       <c r="H15" s="14"/>
     </row>
     <row r="16" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A16" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="6" t="s">
-        <v>23</v>
-      </c>
       <c r="C16" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D16" s="7">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="E16" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F16" s="7">
         <f t="shared" si="0"/>
-        <v>48</v>
+        <v>12</v>
       </c>
       <c r="G16" s="23" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H16" s="14"/>
     </row>
     <row r="17" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A17" s="13" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>26</v>
+        <v>22</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>27</v>
       </c>
       <c r="D17" s="7">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E17" s="6">
         <v>1</v>
       </c>
       <c r="F17" s="7">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G17" s="23" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H17" s="14"/>
     </row>
     <row r="18" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A18" s="13" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D18" s="7">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="E18" s="6">
         <v>1</v>
       </c>
       <c r="F18" s="7">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="G18" s="23" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H18" s="14"/>
     </row>
     <row r="19" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A19" s="13" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D19" s="7">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="E19" s="6">
         <v>1</v>
       </c>
       <c r="F19" s="7">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="G19" s="23" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H19" s="14"/>
     </row>
     <row r="20" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A20" s="13" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D20" s="7">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E20" s="6">
         <v>1</v>
       </c>
       <c r="F20" s="7">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="G20" s="23" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H20" s="14"/>
     </row>
     <row r="21" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A21" s="13" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D21" s="7">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E21" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F21" s="7">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G21" s="23" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H21" s="14"/>
     </row>
-    <row r="22" spans="1:8" ht="15" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="13" t="s">
-        <v>37</v>
+        <v>62</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>38</v>
+        <v>63</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>66</v>
       </c>
       <c r="D22" s="7">
-        <v>4</v>
+        <v>69.989999999999995</v>
       </c>
       <c r="E22" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F22" s="7">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>69.989999999999995</v>
       </c>
       <c r="G22" s="23" t="s">
-        <v>86</v>
+        <v>64</v>
       </c>
       <c r="H22" s="14"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="13" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D23" s="7">
-        <v>69.989999999999995</v>
+        <v>17</v>
       </c>
       <c r="E23" s="6">
         <v>1</v>
       </c>
       <c r="F23" s="7">
         <f t="shared" si="0"/>
-        <v>69.989999999999995</v>
+        <v>17</v>
       </c>
       <c r="G23" s="23" t="s">
-        <v>65</v>
+        <v>96</v>
       </c>
       <c r="H23" s="14"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="D24" s="7">
+    <row r="24" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="B24" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E24" s="6">
+      <c r="C24" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="D24" s="18">
+        <v>21.99</v>
+      </c>
+      <c r="E24" s="16">
         <v>1</v>
       </c>
-      <c r="F24" s="7">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="G24" s="23" t="s">
-        <v>98</v>
-      </c>
-      <c r="H24" s="14"/>
-    </row>
-    <row r="25" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="B25" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="C25" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="D25" s="18">
-        <v>21.99</v>
-      </c>
-      <c r="E25" s="16">
-        <v>1</v>
-      </c>
-      <c r="F25" s="18">
+      <c r="F24" s="18">
         <f t="shared" si="0"/>
         <v>21.99</v>
       </c>
-      <c r="G25" s="24"/>
-      <c r="H25" s="19"/>
-    </row>
-    <row r="26" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="27" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="91" t="s">
-        <v>39</v>
-      </c>
-      <c r="B27" s="92"/>
-      <c r="C27" s="92"/>
-      <c r="D27" s="92"/>
-      <c r="E27" s="92"/>
-      <c r="F27" s="92"/>
-      <c r="G27" s="92"/>
-      <c r="H27" s="93"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="19"/>
+    </row>
+    <row r="25" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="26" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="91" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" s="92"/>
+      <c r="C26" s="92"/>
+      <c r="D26" s="92"/>
+      <c r="E26" s="92"/>
+      <c r="F26" s="92"/>
+      <c r="G26" s="92"/>
+      <c r="H26" s="93"/>
+    </row>
+    <row r="27" spans="1:8" ht="18" x14ac:dyDescent="0.3">
+      <c r="A27" s="49" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" s="45" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27" s="46" t="s">
+        <v>31</v>
+      </c>
+      <c r="D27" s="47">
+        <v>3</v>
+      </c>
+      <c r="E27" s="45">
+        <v>2</v>
+      </c>
+      <c r="F27" s="47"/>
+      <c r="G27" s="48" t="s">
+        <v>87</v>
+      </c>
+      <c r="H27" s="50"/>
     </row>
     <row r="28" spans="1:8" ht="18" x14ac:dyDescent="0.3">
-      <c r="A28" s="49" t="s">
-        <v>31</v>
-      </c>
-      <c r="B28" s="45" t="s">
-        <v>23</v>
-      </c>
-      <c r="C28" s="46" t="s">
-        <v>32</v>
-      </c>
-      <c r="D28" s="47">
-        <v>3</v>
-      </c>
-      <c r="E28" s="45">
-        <v>2</v>
-      </c>
-      <c r="F28" s="47"/>
-      <c r="G28" s="48" t="s">
-        <v>89</v>
-      </c>
-      <c r="H28" s="50"/>
-    </row>
-    <row r="29" spans="1:8" ht="18" x14ac:dyDescent="0.3">
-      <c r="A29" s="51" t="s">
-        <v>59</v>
-      </c>
-      <c r="B29" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="C29" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="D29" s="27"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="28" t="s">
-        <v>88</v>
-      </c>
-      <c r="H29" s="52"/>
+      <c r="A28" s="51" t="s">
+        <v>58</v>
+      </c>
+      <c r="B28" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="C28" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="D28" s="27"/>
+      <c r="E28" s="26"/>
+      <c r="F28" s="27"/>
+      <c r="G28" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="H28" s="52"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" s="53" t="s">
+        <v>97</v>
+      </c>
+      <c r="B29" s="29"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="30"/>
+      <c r="G29" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="H29" s="54"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="53" t="s">
@@ -1977,74 +1960,74 @@
       <c r="E30" s="29"/>
       <c r="F30" s="30"/>
       <c r="G30" s="31" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="H30" s="54"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A31" s="53" t="s">
-        <v>101</v>
-      </c>
-      <c r="B31" s="29"/>
-      <c r="C31" s="29"/>
-      <c r="D31" s="30"/>
-      <c r="E31" s="29"/>
-      <c r="F31" s="30"/>
-      <c r="G31" s="31" t="s">
-        <v>96</v>
-      </c>
-      <c r="H31" s="54"/>
-    </row>
-    <row r="32" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="55" t="s">
-        <v>100</v>
-      </c>
-      <c r="B32" s="56"/>
-      <c r="C32" s="56"/>
-      <c r="D32" s="57"/>
-      <c r="E32" s="56"/>
-      <c r="F32" s="57"/>
-      <c r="G32" s="58" t="s">
+    <row r="31" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="55" t="s">
+        <v>98</v>
+      </c>
+      <c r="B31" s="56"/>
+      <c r="C31" s="56"/>
+      <c r="D31" s="57"/>
+      <c r="E31" s="56"/>
+      <c r="F31" s="57"/>
+      <c r="G31" s="58" t="s">
+        <v>93</v>
+      </c>
+      <c r="H31" s="59"/>
+    </row>
+    <row r="32" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="33" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="85" t="s">
+        <v>39</v>
+      </c>
+      <c r="B33" s="86"/>
+      <c r="C33" s="86"/>
+      <c r="D33" s="86"/>
+      <c r="E33" s="86"/>
+      <c r="F33" s="86"/>
+      <c r="G33" s="86"/>
+      <c r="H33" s="87"/>
+    </row>
+    <row r="34" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A34" s="60" t="s">
+        <v>40</v>
+      </c>
+      <c r="B34" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="C34" s="42" t="s">
+        <v>41</v>
+      </c>
+      <c r="D34" s="43">
+        <v>13.99</v>
+      </c>
+      <c r="E34" s="41" t="s">
+        <v>103</v>
+      </c>
+      <c r="F34" s="43"/>
+      <c r="G34" s="44" t="s">
+        <v>92</v>
+      </c>
+      <c r="H34" s="61"/>
+    </row>
+    <row r="35" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A35" s="62" t="s">
+        <v>43</v>
+      </c>
+      <c r="B35" s="32"/>
+      <c r="C35" s="32"/>
+      <c r="D35" s="33"/>
+      <c r="E35" s="32"/>
+      <c r="F35" s="33"/>
+      <c r="G35" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="H32" s="59"/>
-    </row>
-    <row r="33" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="34" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="85" t="s">
-        <v>40</v>
-      </c>
-      <c r="B34" s="86"/>
-      <c r="C34" s="86"/>
-      <c r="D34" s="86"/>
-      <c r="E34" s="86"/>
-      <c r="F34" s="86"/>
-      <c r="G34" s="86"/>
-      <c r="H34" s="87"/>
-    </row>
-    <row r="35" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A35" s="60" t="s">
-        <v>41</v>
-      </c>
-      <c r="B35" s="41" t="s">
-        <v>23</v>
-      </c>
-      <c r="C35" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="D35" s="43">
-        <v>13.99</v>
-      </c>
-      <c r="E35" s="41" t="s">
-        <v>105</v>
-      </c>
-      <c r="F35" s="43"/>
-      <c r="G35" s="44" t="s">
-        <v>94</v>
-      </c>
-      <c r="H35" s="61"/>
-    </row>
-    <row r="36" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H35" s="63"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="62" t="s">
         <v>44</v>
       </c>
@@ -2054,13 +2037,13 @@
       <c r="E36" s="32"/>
       <c r="F36" s="33"/>
       <c r="G36" s="34" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="H36" s="63"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A37" s="62" t="s">
-        <v>45</v>
+      <c r="A37" s="64" t="s">
+        <v>46</v>
       </c>
       <c r="B37" s="32"/>
       <c r="C37" s="32"/>
@@ -2068,154 +2051,143 @@
       <c r="E37" s="32"/>
       <c r="F37" s="33"/>
       <c r="G37" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="H37" s="63"/>
+    </row>
+    <row r="38" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="65" t="s">
+        <v>45</v>
+      </c>
+      <c r="B38" s="66"/>
+      <c r="C38" s="66"/>
+      <c r="D38" s="67"/>
+      <c r="E38" s="66"/>
+      <c r="F38" s="67"/>
+      <c r="G38" s="68" t="s">
         <v>102</v>
       </c>
-      <c r="H37" s="63"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A38" s="64" t="s">
+      <c r="H38" s="69"/>
+    </row>
+    <row r="39" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="40" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="88" t="s">
         <v>47</v>
       </c>
-      <c r="B38" s="32"/>
-      <c r="C38" s="32"/>
-      <c r="D38" s="33"/>
-      <c r="E38" s="32"/>
-      <c r="F38" s="33"/>
-      <c r="G38" s="34" t="s">
-        <v>103</v>
-      </c>
-      <c r="H38" s="63"/>
-    </row>
-    <row r="39" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="65" t="s">
-        <v>46</v>
-      </c>
-      <c r="B39" s="66"/>
-      <c r="C39" s="66"/>
-      <c r="D39" s="67"/>
-      <c r="E39" s="66"/>
-      <c r="F39" s="67"/>
-      <c r="G39" s="68" t="s">
-        <v>104</v>
-      </c>
-      <c r="H39" s="69"/>
-    </row>
-    <row r="40" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="41" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="88" t="s">
+      <c r="B40" s="89"/>
+      <c r="C40" s="89"/>
+      <c r="D40" s="89"/>
+      <c r="E40" s="89"/>
+      <c r="F40" s="89"/>
+      <c r="G40" s="89"/>
+      <c r="H40" s="90"/>
+    </row>
+    <row r="41" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A41" s="70" t="s">
         <v>48</v>
       </c>
-      <c r="B41" s="89"/>
-      <c r="C41" s="89"/>
-      <c r="D41" s="89"/>
-      <c r="E41" s="89"/>
-      <c r="F41" s="89"/>
-      <c r="G41" s="89"/>
-      <c r="H41" s="90"/>
-    </row>
-    <row r="42" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A42" s="70" t="s">
+      <c r="B41" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="C41" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="B42" s="38" t="s">
-        <v>18</v>
-      </c>
-      <c r="C42" s="38" t="s">
+      <c r="D41" s="39">
+        <v>17.989999999999998</v>
+      </c>
+      <c r="E41" s="38">
+        <v>1</v>
+      </c>
+      <c r="F41" s="39"/>
+      <c r="G41" s="40" t="s">
         <v>50</v>
       </c>
-      <c r="D42" s="39">
-        <v>17.989999999999998</v>
-      </c>
-      <c r="E42" s="38">
+      <c r="H41" s="71"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A42" s="72" t="s">
+        <v>51</v>
+      </c>
+      <c r="B42" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="C42" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="D42" s="36">
+        <v>6.45</v>
+      </c>
+      <c r="E42" s="35">
         <v>1</v>
       </c>
-      <c r="F42" s="39"/>
-      <c r="G42" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="H42" s="71"/>
+      <c r="F42" s="36"/>
+      <c r="G42" s="37" t="s">
+        <v>88</v>
+      </c>
+      <c r="H42" s="73"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A43" s="72" t="s">
+      <c r="A43" s="74" t="s">
         <v>52</v>
       </c>
       <c r="B43" s="35" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C43" s="35" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D43" s="36">
-        <v>6.45</v>
+        <v>4.99</v>
       </c>
       <c r="E43" s="35">
         <v>1</v>
       </c>
       <c r="F43" s="36"/>
       <c r="G43" s="37" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H43" s="73"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A44" s="74" t="s">
-        <v>53</v>
-      </c>
-      <c r="B44" s="35" t="s">
-        <v>18</v>
-      </c>
-      <c r="C44" s="35" t="s">
-        <v>54</v>
-      </c>
-      <c r="D44" s="36">
-        <v>4.99</v>
-      </c>
-      <c r="E44" s="35">
-        <v>1</v>
-      </c>
+      <c r="A44" s="75" t="s">
+        <v>55</v>
+      </c>
+      <c r="B44" s="35"/>
+      <c r="C44" s="35"/>
+      <c r="D44" s="36"/>
+      <c r="E44" s="35"/>
       <c r="F44" s="36"/>
       <c r="G44" s="37" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="H44" s="73"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" s="75" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B45" s="35"/>
       <c r="C45" s="35"/>
       <c r="D45" s="36"/>
       <c r="E45" s="35"/>
       <c r="F45" s="36"/>
-      <c r="G45" s="37" t="s">
-        <v>106</v>
-      </c>
+      <c r="G45" s="37"/>
       <c r="H45" s="73"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A46" s="75" t="s">
-        <v>58</v>
-      </c>
-      <c r="B46" s="35"/>
-      <c r="C46" s="35"/>
-      <c r="D46" s="36"/>
-      <c r="E46" s="35"/>
-      <c r="F46" s="36"/>
-      <c r="G46" s="37"/>
-      <c r="H46" s="73"/>
-    </row>
-    <row r="47" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="76" t="s">
-        <v>57</v>
-      </c>
-      <c r="B47" s="77"/>
-      <c r="C47" s="77"/>
-      <c r="D47" s="78"/>
-      <c r="E47" s="77"/>
-      <c r="F47" s="78"/>
-      <c r="G47" s="79"/>
-      <c r="H47" s="80"/>
+    <row r="46" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="76" t="s">
+        <v>56</v>
+      </c>
+      <c r="B46" s="77"/>
+      <c r="C46" s="77"/>
+      <c r="D46" s="78"/>
+      <c r="E46" s="77"/>
+      <c r="F46" s="78"/>
+      <c r="G46" s="79"/>
+      <c r="H46" s="80"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D47" s="2"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D48" s="2"/>
@@ -2234,16 +2206,13 @@
     </row>
     <row r="53" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D53" s="2"/>
-    </row>
-    <row r="54" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D54" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A34:H34"/>
-    <mergeCell ref="A41:H41"/>
-    <mergeCell ref="A27:H27"/>
+    <mergeCell ref="A33:H33"/>
+    <mergeCell ref="A40:H40"/>
+    <mergeCell ref="A26:H26"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A4" r:id="rId1" xr:uid="{E0B9D346-82E6-4454-BB15-8EEC4E3472B3}"/>
@@ -2253,32 +2222,31 @@
     <hyperlink ref="A7" r:id="rId5" xr:uid="{C777F419-F6D6-4839-ADE3-9D3CC580A9A0}"/>
     <hyperlink ref="A8" r:id="rId6" xr:uid="{3B5E2438-E377-447A-89A7-005593CD72E0}"/>
     <hyperlink ref="A10" r:id="rId7" xr:uid="{2C72E92E-F1DB-4943-A94D-BF25F93C98A5}"/>
-    <hyperlink ref="A11" r:id="rId8" xr:uid="{9C40534E-1A70-4398-B2BF-576716D8F161}"/>
-    <hyperlink ref="A13" r:id="rId9" xr:uid="{0AEC0617-D886-4385-BD4B-8F509CF82AAA}"/>
-    <hyperlink ref="A15" r:id="rId10" xr:uid="{D93BBF9B-964D-4F4B-95F6-99FCCFADE3FB}"/>
-    <hyperlink ref="A18" r:id="rId11" xr:uid="{635EC579-FE8E-4C86-BE11-401C03AE77D1}"/>
-    <hyperlink ref="A19" r:id="rId12" xr:uid="{023383FC-229D-4C7E-AEE3-DB1F332F8B1E}"/>
-    <hyperlink ref="A16" r:id="rId13" xr:uid="{01B0B25D-780F-4456-AF4E-1953A35B88C0}"/>
-    <hyperlink ref="A17" r:id="rId14" xr:uid="{36BEF4B1-C22A-4323-BDFB-39163AEFD519}"/>
-    <hyperlink ref="A20" r:id="rId15" xr:uid="{3A1AFEA7-264C-4020-8F7E-62B80DB7D2BE}"/>
-    <hyperlink ref="A21" r:id="rId16" xr:uid="{2E0F097F-92E7-4E01-AC6B-D2206BB40A7A}"/>
-    <hyperlink ref="A22" r:id="rId17" xr:uid="{10C594D4-14A3-4741-B717-83052185FEA2}"/>
-    <hyperlink ref="A35" r:id="rId18" xr:uid="{EFEC596A-A859-45C9-B449-B01D28E35B03}"/>
-    <hyperlink ref="A42" r:id="rId19" xr:uid="{F62E95EC-7351-4F85-A428-89DE192C8D51}"/>
-    <hyperlink ref="A43" r:id="rId20" xr:uid="{49FA5642-7626-4938-9193-15838A40663D}"/>
-    <hyperlink ref="A44" r:id="rId21" xr:uid="{6AD9CC1F-D06C-4A23-8BF0-FE99D2E1252B}"/>
-    <hyperlink ref="A12" r:id="rId22" xr:uid="{DB5C518D-15FA-4204-8BC2-54930BF3B26C}"/>
-    <hyperlink ref="A23" r:id="rId23" xr:uid="{8EE85784-085F-4688-ADC8-AA7284874CB0}"/>
-    <hyperlink ref="A24" r:id="rId24" xr:uid="{3208E0D2-CB66-4555-BEBD-A74C92F02198}"/>
-    <hyperlink ref="A14" r:id="rId25" xr:uid="{61C10C14-0B88-4C20-8A08-A6C3B4DF4A0D}"/>
-    <hyperlink ref="A31" r:id="rId26" display="AA Batteries " xr:uid="{3B42B57C-45AE-4882-963A-0FBA125919A9}"/>
-    <hyperlink ref="A32" r:id="rId27" display="Kester 0.8mm Rosin Core Solder" xr:uid="{C398C1EC-55BA-4CCD-84EC-3838698C2676}"/>
-    <hyperlink ref="A36" r:id="rId28" xr:uid="{B8FD3279-53D4-4426-83C7-BD61CC0ABDF0}"/>
-    <hyperlink ref="A37" r:id="rId29" xr:uid="{FC28907E-1229-4D42-92B6-9ABD93CFAE70}"/>
-    <hyperlink ref="A28" r:id="rId30" xr:uid="{C0A14886-01A4-4F3F-AE30-F712E50A7925}"/>
-    <hyperlink ref="A25" r:id="rId31" xr:uid="{9C4A64D6-9CA5-4F0E-AB1D-71E88779E7A6}"/>
+    <hyperlink ref="A12" r:id="rId8" xr:uid="{0AEC0617-D886-4385-BD4B-8F509CF82AAA}"/>
+    <hyperlink ref="A14" r:id="rId9" xr:uid="{D93BBF9B-964D-4F4B-95F6-99FCCFADE3FB}"/>
+    <hyperlink ref="A17" r:id="rId10" xr:uid="{635EC579-FE8E-4C86-BE11-401C03AE77D1}"/>
+    <hyperlink ref="A18" r:id="rId11" xr:uid="{023383FC-229D-4C7E-AEE3-DB1F332F8B1E}"/>
+    <hyperlink ref="A15" r:id="rId12" xr:uid="{01B0B25D-780F-4456-AF4E-1953A35B88C0}"/>
+    <hyperlink ref="A16" r:id="rId13" xr:uid="{36BEF4B1-C22A-4323-BDFB-39163AEFD519}"/>
+    <hyperlink ref="A19" r:id="rId14" xr:uid="{3A1AFEA7-264C-4020-8F7E-62B80DB7D2BE}"/>
+    <hyperlink ref="A20" r:id="rId15" xr:uid="{2E0F097F-92E7-4E01-AC6B-D2206BB40A7A}"/>
+    <hyperlink ref="A21" r:id="rId16" xr:uid="{10C594D4-14A3-4741-B717-83052185FEA2}"/>
+    <hyperlink ref="A34" r:id="rId17" xr:uid="{EFEC596A-A859-45C9-B449-B01D28E35B03}"/>
+    <hyperlink ref="A41" r:id="rId18" xr:uid="{F62E95EC-7351-4F85-A428-89DE192C8D51}"/>
+    <hyperlink ref="A42" r:id="rId19" xr:uid="{49FA5642-7626-4938-9193-15838A40663D}"/>
+    <hyperlink ref="A43" r:id="rId20" xr:uid="{6AD9CC1F-D06C-4A23-8BF0-FE99D2E1252B}"/>
+    <hyperlink ref="A11" r:id="rId21" xr:uid="{DB5C518D-15FA-4204-8BC2-54930BF3B26C}"/>
+    <hyperlink ref="A22" r:id="rId22" xr:uid="{8EE85784-085F-4688-ADC8-AA7284874CB0}"/>
+    <hyperlink ref="A23" r:id="rId23" xr:uid="{3208E0D2-CB66-4555-BEBD-A74C92F02198}"/>
+    <hyperlink ref="A13" r:id="rId24" xr:uid="{61C10C14-0B88-4C20-8A08-A6C3B4DF4A0D}"/>
+    <hyperlink ref="A30" r:id="rId25" display="AA Batteries " xr:uid="{3B42B57C-45AE-4882-963A-0FBA125919A9}"/>
+    <hyperlink ref="A31" r:id="rId26" display="Kester 0.8mm Rosin Core Solder" xr:uid="{C398C1EC-55BA-4CCD-84EC-3838698C2676}"/>
+    <hyperlink ref="A35" r:id="rId27" xr:uid="{B8FD3279-53D4-4426-83C7-BD61CC0ABDF0}"/>
+    <hyperlink ref="A36" r:id="rId28" xr:uid="{FC28907E-1229-4D42-92B6-9ABD93CFAE70}"/>
+    <hyperlink ref="A27" r:id="rId29" xr:uid="{C0A14886-01A4-4F3F-AE30-F712E50A7925}"/>
+    <hyperlink ref="A24" r:id="rId30" xr:uid="{9C4A64D6-9CA5-4F0E-AB1D-71E88779E7A6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId32"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId31"/>
 </worksheet>
 </file>
</xml_diff>